<commit_message>
LOTS of generated files
</commit_message>
<xml_diff>
--- a/pythia_ig/output/StructureDefinition-Vaccine.xlsx
+++ b/pythia_ig/output/StructureDefinition-Vaccine.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://fhirfli.dev/fhir/ig/cdsi/StructureDefinition/Vaccine</t>
+    <t>http://fhirfli.dev/fhir/ig/pythia/StructureDefinition/Vaccine</t>
   </si>
   <si>
     <t>Version</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-18T10:38:20+02:00</t>
+    <t>2024-04-29T11:15:56-04:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>